<commit_message>
TD-7294 Issues in notes upload error management
</commit_message>
<xml_diff>
--- a/test/fixtures/xlsx/upload.xlsx
+++ b/test/fixtures/xlsx/upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28521"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\MI1PEPF00000233\EXCELCNV\336b8ff4-ec8a-47a4-94b3-4a8e35042194\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maitane.portilla/workspace/truedat/back/td-dd/test/fixtures/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{458C18A8-FD74-428A-A64F-3EB3BA7538CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A920847E-77B7-491F-87FC-15C0E698DF28}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B237B5ED-E196-E143-AB65-4B72A46417FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" activeTab="1" xr2:uid="{B8937F61-F642-452D-B8D3-6F6A7BFC6533}"/>
+    <workbookView xWindow="80" yWindow="760" windowWidth="30080" windowHeight="18880" xr2:uid="{B8937F61-F642-452D-B8D3-6F6A7BFC6533}"/>
   </bookViews>
   <sheets>
     <sheet name="type_1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="153">
   <si>
     <t>external_id</t>
   </si>
@@ -120,12 +120,363 @@
     <t>system &gt; structure_2</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ex_id6</t>
+  </si>
+  <si>
+    <t>I'm 6</t>
+  </si>
+  <si>
+    <t>structure_4</t>
+  </si>
+  <si>
+    <t>tech_structure_4</t>
+  </si>
+  <si>
+    <t>alias_structure_4</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/4</t>
+  </si>
+  <si>
+    <t>system &gt; structure_4</t>
+  </si>
+  <si>
+    <t>ex_id7</t>
+  </si>
+  <si>
+    <t>Enriched text</t>
+  </si>
+  <si>
+    <t>https://www.google.es</t>
+  </si>
+  <si>
+    <t>structure_5</t>
+  </si>
+  <si>
+    <t>tech_structure_5</t>
+  </si>
+  <si>
+    <t>alias_structure_5</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/5</t>
+  </si>
+  <si>
+    <t>system &gt; structure_5</t>
+  </si>
+  <si>
+    <t>ex_id8</t>
+  </si>
+  <si>
+    <t>structure_6</t>
+  </si>
+  <si>
+    <t>tech_structure_6</t>
+  </si>
+  <si>
+    <t>alias_structure_6</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/6</t>
+  </si>
+  <si>
+    <t>system &gt; structure_6</t>
+  </si>
+  <si>
+    <t>structure_7</t>
+  </si>
+  <si>
+    <t>tech_structure_7</t>
+  </si>
+  <si>
+    <t>alias_structure_7</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/7</t>
+  </si>
+  <si>
+    <t>system &gt; structure_7</t>
+  </si>
+  <si>
+    <t>structure_8</t>
+  </si>
+  <si>
+    <t>tech_structure_8</t>
+  </si>
+  <si>
+    <t>alias_structure_8</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/8</t>
+  </si>
+  <si>
+    <t>system &gt; structure_8</t>
+  </si>
+  <si>
+    <t>I'm 9</t>
+  </si>
+  <si>
+    <t>structure_9</t>
+  </si>
+  <si>
+    <t>tech_structure_9</t>
+  </si>
+  <si>
+    <t>alias_structure_9</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/9</t>
+  </si>
+  <si>
+    <t>system &gt; structure_9</t>
+  </si>
+  <si>
+    <t>ex_id10</t>
+  </si>
+  <si>
+    <t>structure_10</t>
+  </si>
+  <si>
+    <t>tech_structure_10</t>
+  </si>
+  <si>
+    <t>alias_structure_10</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/10</t>
+  </si>
+  <si>
+    <t>system &gt; structure_10</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>key_value</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>hierarchy_name_1</t>
+  </si>
+  <si>
+    <t>hierarchy_name_2</t>
+  </si>
+  <si>
+    <t>ex_id11</t>
+  </si>
+  <si>
+    <t>Role|Role 1</t>
+  </si>
+  <si>
+    <t>structure_11</t>
+  </si>
+  <si>
+    <t>tech_structure_11</t>
+  </si>
+  <si>
+    <t>alias_structure_11</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/11</t>
+  </si>
+  <si>
+    <t>type_2</t>
+  </si>
+  <si>
+    <t>system &gt; structure_11</t>
+  </si>
+  <si>
+    <t>ex_id12</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>structure_12</t>
+  </si>
+  <si>
+    <t>tech_structure_12</t>
+  </si>
+  <si>
+    <t>alias_structure_12</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/12</t>
+  </si>
+  <si>
+    <t>system &gt; structure_12</t>
+  </si>
+  <si>
+    <t>ex_id13</t>
+  </si>
+  <si>
+    <t>structure_13</t>
+  </si>
+  <si>
+    <t>tech_structure_13</t>
+  </si>
+  <si>
+    <t>alias_structure_13</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/13</t>
+  </si>
+  <si>
+    <t>system &gt; structure_13</t>
+  </si>
+  <si>
+    <t>ex_id14</t>
+  </si>
+  <si>
+    <t>structure_14</t>
+  </si>
+  <si>
+    <t>tech_structure_14</t>
+  </si>
+  <si>
+    <t>alias_structure_14</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/14</t>
+  </si>
+  <si>
+    <t>system &gt; structure_14</t>
+  </si>
+  <si>
+    <t>structure_15</t>
+  </si>
+  <si>
+    <t>tech_structure_15</t>
+  </si>
+  <si>
+    <t>alias_structure_15</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/15</t>
+  </si>
+  <si>
+    <t>system &gt; structure_15</t>
+  </si>
+  <si>
+    <t>ex_id16</t>
+  </si>
+  <si>
+    <t>Miss This</t>
+  </si>
+  <si>
+    <t>structure_16</t>
+  </si>
+  <si>
+    <t>tech_structure_16</t>
+  </si>
+  <si>
+    <t>alias_structure_16</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/16</t>
+  </si>
+  <si>
+    <t>system &gt; structure_16</t>
+  </si>
+  <si>
+    <t>ex_id17</t>
+  </si>
+  <si>
+    <t>Role 1</t>
+  </si>
+  <si>
+    <t>structure_17</t>
+  </si>
+  <si>
+    <t>tech_structure_17</t>
+  </si>
+  <si>
+    <t>alias_structure_17</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/17</t>
+  </si>
+  <si>
+    <t>system &gt; structure_17</t>
+  </si>
+  <si>
+    <t>ex_id18</t>
+  </si>
+  <si>
+    <t>Role 2</t>
+  </si>
+  <si>
+    <t>Elemento 2</t>
+  </si>
+  <si>
+    <t>structure_18</t>
+  </si>
+  <si>
+    <t>tech_structure_18</t>
+  </si>
+  <si>
+    <t>alias_structure_18</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/18</t>
+  </si>
+  <si>
+    <t>system &gt; structure_18</t>
+  </si>
+  <si>
+    <t>ex_id19</t>
+  </si>
+  <si>
+    <t>structure_19</t>
+  </si>
+  <si>
+    <t>tech_structure_19</t>
+  </si>
+  <si>
+    <t>alias_structure_19</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/19</t>
+  </si>
+  <si>
+    <t>system &gt; structure_19</t>
+  </si>
+  <si>
+    <t>ex_id20</t>
+  </si>
+  <si>
+    <t>children_1</t>
+  </si>
+  <si>
+    <t>children_1|father</t>
+  </si>
+  <si>
+    <t>structure_20</t>
+  </si>
+  <si>
+    <t>tech_structure_20</t>
+  </si>
+  <si>
+    <t>alias_structure_20</t>
+  </si>
+  <si>
+    <t>http://test.truedat.io/structures/20</t>
+  </si>
+  <si>
+    <t>system &gt; structure_20</t>
+  </si>
+  <si>
+    <t>ex_id15_invalid</t>
+  </si>
+  <si>
     <t>ex_id3</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>structure_3</t>
   </si>
   <si>
@@ -135,377 +486,23 @@
     <t>alias_structure_3</t>
   </si>
   <si>
+    <t>system &gt; structure_3</t>
+  </si>
+  <si>
     <t>http://test.truedat.io/structures/3</t>
   </si>
   <si>
-    <t>system &gt; structure_3</t>
-  </si>
-  <si>
-    <t>ex_id6</t>
-  </si>
-  <si>
-    <t>I'm 6</t>
-  </si>
-  <si>
-    <t>structure_4</t>
-  </si>
-  <si>
-    <t>tech_structure_4</t>
-  </si>
-  <si>
-    <t>alias_structure_4</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/4</t>
-  </si>
-  <si>
-    <t>system &gt; structure_4</t>
-  </si>
-  <si>
-    <t>ex_id7</t>
-  </si>
-  <si>
-    <t>Enriched text</t>
-  </si>
-  <si>
-    <t>https://www.google.es</t>
-  </si>
-  <si>
-    <t>structure_5</t>
-  </si>
-  <si>
-    <t>tech_structure_5</t>
-  </si>
-  <si>
-    <t>alias_structure_5</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/5</t>
-  </si>
-  <si>
-    <t>system &gt; structure_5</t>
-  </si>
-  <si>
-    <t>ex_id8</t>
-  </si>
-  <si>
-    <t>structure_6</t>
-  </si>
-  <si>
-    <t>tech_structure_6</t>
-  </si>
-  <si>
-    <t>alias_structure_6</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/6</t>
-  </si>
-  <si>
-    <t>system &gt; structure_6</t>
+    <t>ex_id9_invalid</t>
   </si>
   <si>
     <t>ex_id4</t>
-  </si>
-  <si>
-    <t>structure_7</t>
-  </si>
-  <si>
-    <t>tech_structure_7</t>
-  </si>
-  <si>
-    <t>alias_structure_7</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/7</t>
-  </si>
-  <si>
-    <t>system &gt; structure_7</t>
-  </si>
-  <si>
-    <t>ex_id5</t>
-  </si>
-  <si>
-    <t>structure_8</t>
-  </si>
-  <si>
-    <t>tech_structure_8</t>
-  </si>
-  <si>
-    <t>alias_structure_8</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/8</t>
-  </si>
-  <si>
-    <t>system &gt; structure_8</t>
-  </si>
-  <si>
-    <t>ex_id9</t>
-  </si>
-  <si>
-    <t>I'm 9</t>
-  </si>
-  <si>
-    <t>structure_9</t>
-  </si>
-  <si>
-    <t>tech_structure_9</t>
-  </si>
-  <si>
-    <t>alias_structure_9</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/9</t>
-  </si>
-  <si>
-    <t>system &gt; structure_9</t>
-  </si>
-  <si>
-    <t>ex_id10</t>
-  </si>
-  <si>
-    <t>structure_10</t>
-  </si>
-  <si>
-    <t>tech_structure_10</t>
-  </si>
-  <si>
-    <t>alias_structure_10</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/10</t>
-  </si>
-  <si>
-    <t>system &gt; structure_10</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>key_value</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>hierarchy_name_1</t>
-  </si>
-  <si>
-    <t>hierarchy_name_2</t>
-  </si>
-  <si>
-    <t>ex_id11</t>
-  </si>
-  <si>
-    <t>Role|Role 1</t>
-  </si>
-  <si>
-    <t>structure_11</t>
-  </si>
-  <si>
-    <t>tech_structure_11</t>
-  </si>
-  <si>
-    <t>alias_structure_11</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/11</t>
-  </si>
-  <si>
-    <t>type_2</t>
-  </si>
-  <si>
-    <t>system &gt; structure_11</t>
-  </si>
-  <si>
-    <t>ex_id12</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>structure_12</t>
-  </si>
-  <si>
-    <t>tech_structure_12</t>
-  </si>
-  <si>
-    <t>alias_structure_12</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/12</t>
-  </si>
-  <si>
-    <t>system &gt; structure_12</t>
-  </si>
-  <si>
-    <t>ex_id13</t>
-  </si>
-  <si>
-    <t>structure_13</t>
-  </si>
-  <si>
-    <t>tech_structure_13</t>
-  </si>
-  <si>
-    <t>alias_structure_13</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/13</t>
-  </si>
-  <si>
-    <t>system &gt; structure_13</t>
-  </si>
-  <si>
-    <t>ex_id14</t>
-  </si>
-  <si>
-    <t>structure_14</t>
-  </si>
-  <si>
-    <t>tech_structure_14</t>
-  </si>
-  <si>
-    <t>alias_structure_14</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/14</t>
-  </si>
-  <si>
-    <t>system &gt; structure_14</t>
-  </si>
-  <si>
-    <t>ex_id15</t>
-  </si>
-  <si>
-    <t>structure_15</t>
-  </si>
-  <si>
-    <t>tech_structure_15</t>
-  </si>
-  <si>
-    <t>alias_structure_15</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/15</t>
-  </si>
-  <si>
-    <t>system &gt; structure_15</t>
-  </si>
-  <si>
-    <t>ex_id16</t>
-  </si>
-  <si>
-    <t>Miss This</t>
-  </si>
-  <si>
-    <t>structure_16</t>
-  </si>
-  <si>
-    <t>tech_structure_16</t>
-  </si>
-  <si>
-    <t>alias_structure_16</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/16</t>
-  </si>
-  <si>
-    <t>system &gt; structure_16</t>
-  </si>
-  <si>
-    <t>ex_id17</t>
-  </si>
-  <si>
-    <t>Role 1</t>
-  </si>
-  <si>
-    <t>structure_17</t>
-  </si>
-  <si>
-    <t>tech_structure_17</t>
-  </si>
-  <si>
-    <t>alias_structure_17</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/17</t>
-  </si>
-  <si>
-    <t>system &gt; structure_17</t>
-  </si>
-  <si>
-    <t>ex_id18</t>
-  </si>
-  <si>
-    <t>Role 2</t>
-  </si>
-  <si>
-    <t>Elemento 2</t>
-  </si>
-  <si>
-    <t>structure_18</t>
-  </si>
-  <si>
-    <t>tech_structure_18</t>
-  </si>
-  <si>
-    <t>alias_structure_18</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/18</t>
-  </si>
-  <si>
-    <t>system &gt; structure_18</t>
-  </si>
-  <si>
-    <t>ex_id19</t>
-  </si>
-  <si>
-    <t>structure_19</t>
-  </si>
-  <si>
-    <t>tech_structure_19</t>
-  </si>
-  <si>
-    <t>alias_structure_19</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/19</t>
-  </si>
-  <si>
-    <t>system &gt; structure_19</t>
-  </si>
-  <si>
-    <t>ex_id20</t>
-  </si>
-  <si>
-    <t>children_1</t>
-  </si>
-  <si>
-    <t>children_1|father</t>
-  </si>
-  <si>
-    <t>structure_20</t>
-  </si>
-  <si>
-    <t>tech_structure_20</t>
-  </si>
-  <si>
-    <t>alias_structure_20</t>
-  </si>
-  <si>
-    <t>http://test.truedat.io/structures/20</t>
-  </si>
-  <si>
-    <t>system &gt; structure_20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,6 +645,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -946,7 +949,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -990,12 +993,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1027,6 +1032,7 @@
     <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8"/>
     <cellStyle name="Hyperlink" xfId="42" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1054,9 +1060,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1094,7 +1100,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1200,7 +1206,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1342,7 +1348,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1350,29 +1356,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0BD2D9-4B14-4A96-AFA1-1A49034C2CCE}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1474,24 +1480,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>148</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
@@ -1500,27 +1506,27 @@
         <v>18</v>
       </c>
       <c r="L4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
@@ -1529,30 +1535,30 @@
         <v>18</v>
       </c>
       <c r="L5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="I6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -1561,27 +1567,27 @@
         <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
@@ -1590,27 +1596,27 @@
         <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -1619,27 +1625,27 @@
         <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
@@ -1648,27 +1654,27 @@
         <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -1677,24 +1683,24 @@
         <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="J11" t="s">
         <v>9</v>
@@ -1703,21 +1709,52 @@
         <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" t="s">
+        <v>148</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{07295398-9A5A-4D2A-9AFA-5A36F0045934}"/>
     <hyperlink ref="I3" r:id="rId2" xr:uid="{C33D348E-CD30-4897-AB43-285269B5FD05}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{3231AA82-1A0B-4641-8037-80A3726EF415}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{FE004298-10C8-43C0-9CF1-5B022AF129E6}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{B40C7CD3-8874-43EA-BAFB-2811C8ECDC23}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{3A1D3C73-C560-4D7A-A165-F90EFE70EF02}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{8F5455BC-CFE1-4BF1-B0B4-ED520187A28C}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{EDD53C95-05A1-4285-BB59-B9CD61F03D87}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{56005183-91A7-408F-A474-44BB7C742499}"/>
-    <hyperlink ref="I11" r:id="rId10" xr:uid="{A91E18C8-7447-4F20-8F08-F0FF4930EC7E}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{FE004298-10C8-43C0-9CF1-5B022AF129E6}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{B40C7CD3-8874-43EA-BAFB-2811C8ECDC23}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{3A1D3C73-C560-4D7A-A165-F90EFE70EF02}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{8F5455BC-CFE1-4BF1-B0B4-ED520187A28C}"/>
+    <hyperlink ref="I9" r:id="rId7" xr:uid="{EDD53C95-05A1-4285-BB59-B9CD61F03D87}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{56005183-91A7-408F-A474-44BB7C742499}"/>
+    <hyperlink ref="I11" r:id="rId9" xr:uid="{A91E18C8-7447-4F20-8F08-F0FF4930EC7E}"/>
+    <hyperlink ref="I4" r:id="rId10" xr:uid="{1B365222-F2C2-C443-A93C-60668415BE52}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{5E2AA5CB-F382-8741-AA01-A7A5FA6EAE11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1727,43 +1764,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AA5177-8C00-44E0-BC1B-E9FE1A8460CF}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1787,314 +1824,314 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G3" t="s">
         <v>86</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
         <v>87</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I3" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" t="s">
         <v>90</v>
       </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>91</v>
       </c>
-      <c r="M2" t="s">
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
+      <c r="H4" t="s">
         <v>93</v>
       </c>
-      <c r="B3" t="s">
+      <c r="I4" t="s">
         <v>94</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" t="s">
         <v>96</v>
       </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="G5" t="s">
         <v>98</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="H5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="I5" t="s">
         <v>100</v>
       </c>
-      <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="J5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" t="s">
         <v>102</v>
       </c>
-      <c r="I4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" t="s">
-        <v>91</v>
-      </c>
-      <c r="M5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K6" t="s">
         <v>9</v>
       </c>
       <c r="L6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="M6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
+        <v>82</v>
+      </c>
+      <c r="M8" t="s">
         <v>121</v>
       </c>
-      <c r="I7" t="s">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="B9" t="s">
         <v>123</v>
       </c>
-      <c r="K7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" t="s">
-        <v>91</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="C9" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
+      <c r="G9" t="s">
         <v>125</v>
       </c>
-      <c r="B8" t="s">
+      <c r="H9" t="s">
         <v>126</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I9" t="s">
         <v>127</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J9" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" t="s">
+        <v>82</v>
+      </c>
+      <c r="M9" t="s">
         <v>129</v>
       </c>
-      <c r="J8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>130</v>
       </c>
-      <c r="K8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" t="s">
-        <v>91</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
+      <c r="H10" t="s">
         <v>132</v>
       </c>
-      <c r="B9" t="s">
+      <c r="I10" t="s">
         <v>133</v>
       </c>
-      <c r="C9" t="s">
+      <c r="J10" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" t="s">
         <v>135</v>
       </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>136</v>
       </c>
-      <c r="I9" t="s">
+      <c r="E11" t="s">
         <v>137</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="F11" t="s">
         <v>138</v>
       </c>
-      <c r="K9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" t="s">
-        <v>91</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="G11" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
+      <c r="H11" t="s">
         <v>140</v>
       </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="I11" t="s">
         <v>141</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J11" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11" t="s">
         <v>143</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" t="s">
-        <v>91</v>
-      </c>
-      <c r="M10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E11" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" t="s">
-        <v>148</v>
-      </c>
-      <c r="G11" t="s">
-        <v>149</v>
-      </c>
-      <c r="H11" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" t="s">
-        <v>91</v>
-      </c>
-      <c r="M11" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{A15D72AC-A673-444C-9901-4AA32A5804E9}"/>
-    <hyperlink ref="J3" r:id="rId2" display="http://test.truedat.io/structures/11" xr:uid="{83D6609C-75D8-4616-A8AA-2CA8ED729E2E}"/>
-    <hyperlink ref="J4" r:id="rId3" display="http://test.truedat.io/structures/11" xr:uid="{49AFA45F-D638-4CDC-B950-219F032AE116}"/>
-    <hyperlink ref="J5" r:id="rId4" display="http://test.truedat.io/structures/11" xr:uid="{77FE2837-A3C1-4BFF-81A3-3E91E953C7A7}"/>
-    <hyperlink ref="J6" r:id="rId5" display="http://test.truedat.io/structures/11" xr:uid="{64B0B0B9-20F3-419E-9460-D5362ED9789D}"/>
-    <hyperlink ref="J7" r:id="rId6" display="http://test.truedat.io/structures/11" xr:uid="{013E2EEE-2BB5-4129-8254-43B12F1BB33C}"/>
-    <hyperlink ref="J8" r:id="rId7" display="http://test.truedat.io/structures/11" xr:uid="{048ED0B0-E927-4BFB-B71E-15C5CA216AE5}"/>
-    <hyperlink ref="J9" r:id="rId8" display="http://test.truedat.io/structures/11" xr:uid="{58C87865-FDD1-488D-BD4A-AD3CA7CBE3F0}"/>
-    <hyperlink ref="J10" r:id="rId9" display="http://test.truedat.io/structures/11" xr:uid="{6EDD6B5B-F040-4BDD-8B07-F95979BC02A6}"/>
-    <hyperlink ref="J11" r:id="rId10" display="http://test.truedat.io/structures/11" xr:uid="{A72CB661-4C71-4415-8ECB-ED512B10969F}"/>
+    <hyperlink ref="J4" r:id="rId2" display="http://test.truedat.io/structures/11" xr:uid="{49AFA45F-D638-4CDC-B950-219F032AE116}"/>
+    <hyperlink ref="J5" r:id="rId3" display="http://test.truedat.io/structures/11" xr:uid="{77FE2837-A3C1-4BFF-81A3-3E91E953C7A7}"/>
+    <hyperlink ref="J6" r:id="rId4" display="http://test.truedat.io/structures/11" xr:uid="{64B0B0B9-20F3-419E-9460-D5362ED9789D}"/>
+    <hyperlink ref="J7" r:id="rId5" display="http://test.truedat.io/structures/11" xr:uid="{013E2EEE-2BB5-4129-8254-43B12F1BB33C}"/>
+    <hyperlink ref="J8" r:id="rId6" display="http://test.truedat.io/structures/11" xr:uid="{048ED0B0-E927-4BFB-B71E-15C5CA216AE5}"/>
+    <hyperlink ref="J9" r:id="rId7" display="http://test.truedat.io/structures/11" xr:uid="{58C87865-FDD1-488D-BD4A-AD3CA7CBE3F0}"/>
+    <hyperlink ref="J10" r:id="rId8" display="http://test.truedat.io/structures/11" xr:uid="{6EDD6B5B-F040-4BDD-8B07-F95979BC02A6}"/>
+    <hyperlink ref="J11" r:id="rId9" display="http://test.truedat.io/structures/11" xr:uid="{A72CB661-4C71-4415-8ECB-ED512B10969F}"/>
+    <hyperlink ref="J3" r:id="rId10" display="http://test.truedat.io/structures/11" xr:uid="{83D6609C-75D8-4616-A8AA-2CA8ED729E2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>